<commit_message>
Sprint 5 contribution spreadsheet
</commit_message>
<xml_diff>
--- a/Contribution.xlsx
+++ b/Contribution.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lewis\OneDrive\Documents\Uni\Year 3\Group Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ca01c0acc71d382/Documents/Uni/Year 3/Group Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{B8E03C00-A032-45AB-8452-3D4DD1B6429D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9E280954-488D-4CC0-86CA-1EA247020C6B}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{B8E03C00-A032-45AB-8452-3D4DD1B6429D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{616D481C-0CC9-491E-BFA6-A7203420D3FB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -538,7 +538,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -767,28 +767,54 @@
       <c r="A9" s="5">
         <v>9</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="B9" s="6">
+        <v>43906</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.2</v>
+      </c>
       <c r="H9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>10</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="B10" s="6">
+        <v>43913</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0.2</v>
+      </c>
       <c r="H10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -842,27 +868,27 @@
       </c>
       <c r="C15" s="2">
         <f>SUM(C2:C13)/COUNT(C2:C13)</f>
-        <v>0.215</v>
+        <v>0.21166666666666664</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" ref="D15:H15" si="1">SUM(D2:D13)/COUNT(D2:D13)</f>
-        <v>0.18642857142857142</v>
+        <v>0.18944444444444442</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="1"/>
-        <v>0.21071428571428569</v>
+        <v>0.20833333333333331</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="1"/>
-        <v>0.19642857142857142</v>
+        <v>0.19722222222222222</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="1"/>
-        <v>0.19142857142857142</v>
+        <v>0.1933333333333333</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="1"/>
-        <v>0.58333333333333337</v>
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sprint 6 contribution spreadsheet
</commit_message>
<xml_diff>
--- a/Contribution.xlsx
+++ b/Contribution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ca01c0acc71d382/Documents/Uni/Year 3/Group Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="8_{B8E03C00-A032-45AB-8452-3D4DD1B6429D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{616D481C-0CC9-491E-BFA6-A7203420D3FB}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="8_{B8E03C00-A032-45AB-8452-3D4DD1B6429D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D6CD03F8-DE01-4B48-8309-6E2635DCB83F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -538,7 +538,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -821,14 +821,27 @@
       <c r="A11" s="5">
         <v>11</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="B11" s="6">
+        <v>43920</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.2</v>
+      </c>
       <c r="H11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -868,27 +881,27 @@
       </c>
       <c r="C15" s="2">
         <f>SUM(C2:C13)/COUNT(C2:C13)</f>
-        <v>0.21166666666666664</v>
+        <v>0.21049999999999999</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" ref="D15:H15" si="1">SUM(D2:D13)/COUNT(D2:D13)</f>
-        <v>0.18944444444444442</v>
+        <v>0.19049999999999997</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="1"/>
-        <v>0.20833333333333331</v>
+        <v>0.20749999999999996</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="1"/>
-        <v>0.19722222222222222</v>
+        <v>0.19749999999999998</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="1"/>
-        <v>0.1933333333333333</v>
+        <v>0.19399999999999998</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>